<commit_message>
Silver's data no longer borked
</commit_message>
<xml_diff>
--- a/GW2Tradz/GW2Tradz/salvage.xlsx
+++ b/GW2Tradz/GW2Tradz/salvage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krise\Documents\GitHub\GW2Tradz\GW2Tradz\GW2Tradz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A76A25-F462-4223-A990-7E45883BA0F9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1CB6FC8-DE58-44FB-916A-6378A19AAC0B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="1000" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valuable Metal Scrap (Copperfed" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,9 @@
     <sheet name="Discarded Garments (Copperfed)" sheetId="6" r:id="rId6"/>
     <sheet name="Bloodstone-Warped Hides (Silver" sheetId="7" r:id="rId7"/>
     <sheet name="Unstable Metal Chunks (Copperfe" sheetId="10" r:id="rId8"/>
-    <sheet name="Sheet6" sheetId="11" r:id="rId9"/>
-    <sheet name="Hard Leather Straps (Silverfed)" sheetId="9" r:id="rId10"/>
+    <sheet name="Salvageable Fused Metal Scraps " sheetId="11" r:id="rId9"/>
+    <sheet name="Salvageable Metal Scraps (Coppe" sheetId="12" r:id="rId10"/>
+    <sheet name="Hard Leather Straps (Silverfed)" sheetId="9" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
   <si>
     <t>Orichalcum Ore</t>
   </si>
@@ -108,9 +109,6 @@
     <t>Hardened Leather Sections</t>
   </si>
   <si>
-    <t>Rawhide Leather Sections</t>
-  </si>
-  <si>
     <t>Thin Leather Sections</t>
   </si>
   <si>
@@ -142,6 +140,18 @@
   </si>
   <si>
     <t>Glacial Core</t>
+  </si>
+  <si>
+    <t>Salvageable Metal Scraps (Copperfed)</t>
+  </si>
+  <si>
+    <t>Coarse Leather Sections</t>
+  </si>
+  <si>
+    <t>Glacial Lodestone</t>
+  </si>
+  <si>
+    <t>Bloodstone-Warped Hides (Silverfed)2</t>
   </si>
 </sst>
 </file>
@@ -203,17 +213,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C7" totalsRowCount="1">
-  <autoFilter ref="A1:C6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C8" totalsRowCount="1">
+  <autoFilter ref="A1:C7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Valuable Metal Scrap (Copperfed)" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,A2:A6)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,A2:A7)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Mithril Ore" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,B2:B6)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,B2:B7)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Orichalcum Ore" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,C2:C6)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,C2:C7)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -221,98 +231,116 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{436DD24B-6473-49CB-BC2B-2C5E70B741F9}" name="Table167849" displayName="Table167849" ref="A1:C3" totalsRowCount="1">
-  <autoFilter ref="A1:C2" xr:uid="{435B9412-207A-46D7-85DB-63D3D0B190BE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{E5E7FB19-106A-4512-B469-28100BDD1999}" name="Table16784141516" displayName="Table16784141516" ref="A1:C4" totalsRowCount="1">
+  <autoFilter ref="A1:C3" xr:uid="{E1E674C0-644D-4043-A0DA-8F6C9A034074}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{C5B20C03-6A20-46E2-9028-19F64A37B316}" name="Hard Leather Straps (Silverfed)" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,A2:A2)</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="2" xr3:uid="{C9486A08-89B2-4526-8B62-626FA437DDFD}" name="Thick Leather Sections" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,B2:B2)</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{A990BAC9-4FF6-4D60-8E56-7D2131F5A3D5}" name="Hardened Leather Sections" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,C2:C2)</totalsRowFormula>
+    <tableColumn id="1" xr3:uid="{D0F91126-0432-42C1-98B7-5CF135044FD4}" name="Salvageable Metal Scraps (Copperfed)" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(109,A2:A3)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{905B65C4-0EA7-4FDB-8C52-E325EC4F221A}" name="Mithril Ore" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(109,B2:B3)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{A4C94530-5721-4643-A7CE-B63AEB5E922C}" name="Platinum Ore" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(109,C2:C3)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table15" displayName="Table15" ref="A1:D5" totalsRowCount="1">
-  <autoFilter ref="A1:D4" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Salvageable Intact Forged Scrap (Copperfed)" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,A2:A4)</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Mithril Ore" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,B2:B4)</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Orichalcum Ore" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,C2:C4)</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Slivers of Twisting Forgemetal" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,D2:D4)</totalsRowFormula>
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{436DD24B-6473-49CB-BC2B-2C5E70B741F9}" name="Table167849" displayName="Table167849" ref="A1:C4" totalsRowCount="1">
+  <autoFilter ref="A1:C3" xr:uid="{435B9412-207A-46D7-85DB-63D3D0B190BE}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{C5B20C03-6A20-46E2-9028-19F64A37B316}" name="Hard Leather Straps (Silverfed)" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(109,A2:A3)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{C9486A08-89B2-4526-8B62-626FA437DDFD}" name="Thick Leather Sections" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(109,B2:B3)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{A990BAC9-4FF6-4D60-8E56-7D2131F5A3D5}" name="Hardened Leather Sections" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(109,C2:C3)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table16" displayName="Table16" ref="A1:B3" totalsRowCount="1">
-  <autoFilter ref="A1:B2" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Lump of Raw Ambrite (Copperfed)" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,A2:A2)</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Pieces of Ambrite" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,B2:B2)</totalsRowFormula>
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table15" displayName="Table15" ref="A1:D6" totalsRowCount="1">
+  <autoFilter ref="A1:D5" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Salvageable Intact Forged Scrap (Copperfed)" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(109,A2:A5)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Mithril Ore" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(109,B2:B5)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Orichalcum Ore" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(109,C2:C5)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Slivers of Twisting Forgemetal" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(109,D2:D5)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table167" displayName="Table167" ref="A1:B3" totalsRowCount="1">
-  <autoFilter ref="A1:B2" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table16" displayName="Table16" ref="A1:B4" totalsRowCount="1">
+  <autoFilter ref="A1:B3" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Glob of Ectoplasm (Silverfed)" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,A2:A2)</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Pile of Crystalline Dust" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,B2:B2)</totalsRowFormula>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Lump of Raw Ambrite (Copperfed)" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(109,A2:A3)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Pieces of Ambrite" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(109,B2:B3)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table167" displayName="Table167" ref="A1:B4" totalsRowCount="1">
+  <autoFilter ref="A1:B3" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Glob of Ectoplasm (Silverfed)" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(109,A2:A3)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Pile of Crystalline Dust" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(109,B2:B3)</totalsRowFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table1678" displayName="Table1678" ref="A1:G4" totalsRowCount="1">
-  <autoFilter ref="A1:G3" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table1678" displayName="Table1678" ref="A1:G5" totalsRowCount="1">
+  <autoFilter ref="A1:G4" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Reclaimed Wood Chunk (Copperfed)" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,A2:A3)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,A2:A4)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Green Wood Log" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,B2:B3)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,B2:B4)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Soft Wood Logs" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,C2:C3)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,C2:C4)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Seasoned Wood Logs" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,D2:D3)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,D2:D4)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Hard Wood Logs" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,E2:E3)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,E2:E4)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Elder Wood Logs " totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,F2:F3)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,F2:F4)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="Ancient Wood Logs" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,G2:G3)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,G2:G4)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -338,29 +366,32 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6683A40A-984F-4C8C-B5BD-CEDCA44A00C1}" name="Table16784" displayName="Table16784" ref="A1:G3" totalsRowCount="1">
-  <autoFilter ref="A1:G2" xr:uid="{25A4AE94-A8F7-4B52-994F-DE080FA22BF0}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6683A40A-984F-4C8C-B5BD-CEDCA44A00C1}" name="Table16784" displayName="Table16784" ref="A1:H3" insertRow="1" totalsRowCount="1">
+  <autoFilter ref="A1:H2" xr:uid="{25A4AE94-A8F7-4B52-994F-DE080FA22BF0}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{C9ADA6AC-04B8-418E-8FE6-FC3F390007F7}" name="Bloodstone-Warped Hides (Silverfed)" totalsRowFunction="custom">
       <totalsRowFormula>SUBTOTAL(109,A2:A2)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{197B031B-E04A-4D3A-964A-24491C36C27D}" name="Rawhide Leather Sections" totalsRowFunction="custom">
+    <tableColumn id="2" xr3:uid="{197B031B-E04A-4D3A-964A-24491C36C27D}" name="Bloodstone-Warped Hides (Silverfed)2" totalsRowFunction="custom">
       <totalsRowFormula>SUBTOTAL(109,B2:B2)</totalsRowFormula>
     </tableColumn>
+    <tableColumn id="3" xr3:uid="{85DBBF6B-7DBD-4ED0-A92A-18C784047461}" name="Coarse Leather Sections" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(109,C2:C2)</totalsRowFormula>
+    </tableColumn>
     <tableColumn id="4" xr3:uid="{EB728ABA-20A8-45CC-B029-FADB42BA26B9}" name="Thin Leather Sections" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,C2:C2)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,D2:D2)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{602D6133-C0B4-4E0B-8CCC-39EA2C037EEB}" name="Rugged Leather Sections" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,D2:D2)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,E2:E2)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{388DB14A-54F3-4CB4-9FAC-CC79EC380AB9}" name="Hard Wood Logs" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,E2:E2)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,F2:F2)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{9D638586-026B-44D1-8B34-C0C3D43CAD18}" name="Thick Leather Sections" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,F2:F2)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,G2:G2)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{8CF9AEA9-3895-4903-8246-88658B570EA4}" name="Hardened Leather Sections" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,G2:G2)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,H2:H2)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -368,26 +399,26 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{5DA2CE26-8E50-4E72-9C9C-77AF18B12840}" name="Table1678414" displayName="Table1678414" ref="A1:F3" totalsRowCount="1">
-  <autoFilter ref="A1:F2" xr:uid="{161BA580-722A-410D-8E2D-E64F92884D13}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{5DA2CE26-8E50-4E72-9C9C-77AF18B12840}" name="Table1678414" displayName="Table1678414" ref="A1:F4" totalsRowCount="1">
+  <autoFilter ref="A1:F3" xr:uid="{161BA580-722A-410D-8E2D-E64F92884D13}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{6C2025F3-98C0-40DF-AF82-32553C5F93DE}" name="Unstable Metal Chunks (Copperfed)" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,A2:A2)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,A2:A3)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{80F128D0-8E55-4315-89EA-72129B453E33}" name="Copper Ore" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,B2:B2)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,B2:B3)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{68879772-4267-45A2-B3E5-F3965BE06DBE}" name="Iron Ore" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,C2:C2)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,C2:C3)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{4BFE3333-64CA-45C6-BD5C-ED96D1041663}" name="Platinum Ore" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,D2:D2)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,D2:D3)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{7AEC54C7-90D4-4B3E-9B16-536F9AD35119}" name="Mithril Ore" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,E2:E2)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,E2:E3)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{0C6CECE8-CF3F-4FD2-BCB2-8948DCAAE7D6}" name="Orichalcum Ore" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,F2:F2)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,F2:F3)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -395,26 +426,29 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{8CE988A0-C50E-4CC4-88CD-D3F5FB332B81}" name="Table167841415" displayName="Table167841415" ref="A1:F3" totalsRowCount="1">
-  <autoFilter ref="A1:F2" xr:uid="{7CCC29B3-4E29-4434-9033-BB5CD6A1C02E}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{8CE988A0-C50E-4CC4-88CD-D3F5FB332B81}" name="Table167841415" displayName="Table167841415" ref="A1:G4" totalsRowCount="1">
+  <autoFilter ref="A1:G3" xr:uid="{7CCC29B3-4E29-4434-9033-BB5CD6A1C02E}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{21B805E5-8EF4-4B33-B45E-03CB622F6AD3}" name="Salvageable Fused Metal Scraps (Copperfed)" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,A2:A2)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,A2:A3)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{28F7B35D-F3F2-4F5D-A14A-5C0A1E59AB96}" name="Molten Core" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,B2:B2)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,B2:B3)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{62CCA669-CBD2-4DE6-84EC-17BB481C9C91}" name="Molten Lodestone" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,C2:C2)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,C2:C3)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{9556E610-E477-4966-A066-9B2695745F6E}" name="Glacial Core" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,D2:D2)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,D2:D3)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{80E8700E-CFC1-4F90-8331-94C026EE1108}" name="Glacial Lodestone" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(109,E2:E3)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{F1F3AD18-1C24-4218-9CCF-1CD3124E3CB8}" name="Mithril Ore" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,E2:E2)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,F2:F3)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{5C8FFD83-4405-4639-8D5C-AA0C78802CFF}" name="Orichalcum Ore" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,F2:F2)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,G2:G3)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -718,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,41 +823,52 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>6209</v>
+        <v>2687</v>
       </c>
       <c r="B6">
-        <v>7350</v>
+        <v>3223</v>
       </c>
       <c r="C6">
-        <v>1359</v>
+        <v>598</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>SUBTOTAL(109,A2:A6)</f>
-        <v>15031</v>
+        <v>6209</v>
       </c>
       <c r="B7">
-        <f>SUBTOTAL(109,B2:B6)</f>
-        <v>17955</v>
+        <v>7350</v>
       </c>
       <c r="C7">
-        <f>SUBTOTAL(109,C2:C6)</f>
-        <v>3223</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
+        <f>SUBTOTAL(109,A2:A7)</f>
+        <v>17718</v>
+      </c>
+      <c r="B8">
+        <f>SUBTOTAL(109,B2:B7)</f>
+        <v>21178</v>
+      </c>
+      <c r="C8">
+        <f>SUBTOTAL(109,C2:C7)</f>
+        <v>3821</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
         <f>Table1[[#Totals],[Valuable Metal Scrap (Copperfed)]]/Table1[[#Totals],[Valuable Metal Scrap (Copperfed)]]</f>
         <v>1</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <f>Table1[[#Totals],[Mithril Ore]]/Table1[[#Totals],[Valuable Metal Scrap (Copperfed)]]</f>
-        <v>1.1945313019759165</v>
-      </c>
-      <c r="C8">
+        <v>1.1952816344959927</v>
+      </c>
+      <c r="C9">
         <f>Table1[[#Totals],[Orichalcum Ore]]/Table1[[#Totals],[Valuable Metal Scrap (Copperfed)]]</f>
-        <v>0.21442352471558779</v>
+        <v>0.21565639462693306</v>
       </c>
     </row>
   </sheetData>
@@ -835,11 +880,93 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF5987D4-1F44-4781-96D3-48B6972FA2CE}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="77.28515625" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>59</v>
+      </c>
+      <c r="B2">
+        <v>65</v>
+      </c>
+      <c r="C2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>102</v>
+      </c>
+      <c r="B3">
+        <v>115</v>
+      </c>
+      <c r="C3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>SUBTOTAL(109,A2:A3)</f>
+        <v>161</v>
+      </c>
+      <c r="B4">
+        <f>SUBTOTAL(109,B2:B3)</f>
+        <v>180</v>
+      </c>
+      <c r="C4">
+        <f>SUBTOTAL(109,C2:C3)</f>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f>Table16784141516[[#Totals],[Salvageable Metal Scraps (Copperfed)]]/Table16784141516[[#Totals],[Salvageable Metal Scraps (Copperfed)]]</f>
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <f>Table16784141516[[#Totals],[Mithril Ore]]/Table16784141516[[#Totals],[Salvageable Metal Scraps (Copperfed)]]</f>
+        <v>1.1180124223602483</v>
+      </c>
+      <c r="C5">
+        <f>Table16784141516[[#Totals],[Platinum Ore]]/Table16784141516[[#Totals],[Salvageable Metal Scraps (Copperfed)]]</f>
+        <v>0.56521739130434778</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C72D2860-57B6-4373-880B-086D8C6F9373}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,7 +978,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>20</v>
@@ -873,30 +1000,41 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>SUBTOTAL(109,A2:A2)</f>
-        <v>1165</v>
+        <v>1592</v>
       </c>
       <c r="B3">
-        <f>SUBTOTAL(109,B2:B2)</f>
-        <v>1463</v>
+        <v>2030</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3" si="0">SUBTOTAL(109,C2:C2)</f>
-        <v>113</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
+        <f>SUBTOTAL(109,A2:A3)</f>
+        <v>2757</v>
+      </c>
+      <c r="B4">
+        <f>SUBTOTAL(109,B2:B3)</f>
+        <v>3493</v>
+      </c>
+      <c r="C4">
+        <f>SUBTOTAL(109,C2:C3)</f>
+        <v>261</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
         <f>Table167849[[#Totals],[Hard Leather Straps (Silverfed)]]/Table167849[[#Totals],[Hard Leather Straps (Silverfed)]]</f>
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <f>Table167849[[#Totals],[Thick Leather Sections]]/Table167849[[#Totals],[Hard Leather Straps (Silverfed)]]</f>
-        <v>1.255793991416309</v>
-      </c>
-      <c r="C4">
+        <v>1.2669568371418207</v>
+      </c>
+      <c r="C5">
         <f>Table167849[[#Totals],[Hardened Leather Sections]]/Table167849[[#Totals],[Hard Leather Straps (Silverfed)]]</f>
-        <v>9.6995708154506435E-2</v>
+        <v>9.4668117519042444E-2</v>
       </c>
     </row>
   </sheetData>
@@ -909,11 +1047,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -939,80 +1075,94 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>518</v>
+        <v>223</v>
       </c>
       <c r="B2">
-        <v>2169</v>
+        <v>982</v>
       </c>
       <c r="C2">
-        <v>150</v>
+        <v>57</v>
       </c>
       <c r="D2">
-        <v>148</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>322</v>
+        <v>518</v>
       </c>
       <c r="B3">
-        <v>1355</v>
+        <v>2169</v>
       </c>
       <c r="C3">
-        <v>117</v>
+        <v>150</v>
       </c>
       <c r="D3">
-        <v>75</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>491</v>
+        <v>322</v>
       </c>
       <c r="B4">
-        <v>2061</v>
+        <v>1355</v>
       </c>
       <c r="C4">
-        <v>147</v>
+        <v>117</v>
       </c>
       <c r="D4">
-        <v>118</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>SUBTOTAL(109,A2:A4)</f>
-        <v>1331</v>
+        <v>491</v>
       </c>
       <c r="B5">
-        <f>SUBTOTAL(109,B2:B4)</f>
-        <v>5585</v>
+        <v>2061</v>
       </c>
       <c r="C5">
-        <f>SUBTOTAL(109,C2:C4)</f>
-        <v>414</v>
+        <v>147</v>
       </c>
       <c r="D5">
-        <f>SUBTOTAL(109,D2:D4)</f>
-        <v>341</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
+        <f>SUBTOTAL(109,A2:A5)</f>
+        <v>1554</v>
+      </c>
+      <c r="B6">
+        <f>SUBTOTAL(109,B2:B5)</f>
+        <v>6567</v>
+      </c>
+      <c r="C6">
+        <f>SUBTOTAL(109,C2:C5)</f>
+        <v>471</v>
+      </c>
+      <c r="D6">
+        <f>SUBTOTAL(109,D2:D5)</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
         <f>Table15[[#Totals],[Salvageable Intact Forged Scrap (Copperfed)]]/Table15[[#Totals],[Salvageable Intact Forged Scrap (Copperfed)]]</f>
         <v>1</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <f>Table15[[#Totals],[Mithril Ore]]/Table15[[#Totals],[Salvageable Intact Forged Scrap (Copperfed)]]</f>
-        <v>4.1960931630353118</v>
-      </c>
-      <c r="C6">
+        <v>4.2258687258687262</v>
+      </c>
+      <c r="C7">
         <f>Table15[[#Totals],[Orichalcum Ore]]/Table15[[#Totals],[Salvageable Intact Forged Scrap (Copperfed)]]</f>
-        <v>0.31104432757325318</v>
-      </c>
-      <c r="D6">
+        <v>0.30308880308880309</v>
+      </c>
+      <c r="D7">
         <f>Table15[[#Totals],[Slivers of Twisting Forgemetal]]/Table15[[#Totals],[Salvageable Intact Forged Scrap (Copperfed)]]</f>
-        <v>0.256198347107438</v>
+        <v>0.2574002574002574</v>
       </c>
     </row>
   </sheetData>
@@ -1025,7 +1175,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1045,30 +1195,38 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>4500</v>
+        <v>500</v>
       </c>
       <c r="B2">
-        <v>8959</v>
+        <v>986</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>SUBTOTAL(109,A2:A2)</f>
         <v>4500</v>
       </c>
       <c r="B3">
-        <f>SUBTOTAL(109,B2:B2)</f>
         <v>8959</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
+        <f>SUBTOTAL(109,A2:A3)</f>
+        <v>5000</v>
+      </c>
+      <c r="B4">
+        <f>SUBTOTAL(109,B2:B3)</f>
+        <v>9945</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
         <f>Table16[[#Totals],[Lump of Raw Ambrite (Copperfed)]]/Table16[[#Totals],[Lump of Raw Ambrite (Copperfed)]]</f>
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <f>Table16[[#Totals],[Pieces of Ambrite]]/Table16[[#Totals],[Lump of Raw Ambrite (Copperfed)]]</f>
-        <v>1.9908888888888889</v>
+        <v>1.9890000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1081,10 +1239,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1106,27 +1264,35 @@
         <v>500</v>
       </c>
       <c r="B2">
-        <v>949</v>
+        <v>919</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>SUBTOTAL(109,A2:A2)</f>
         <v>500</v>
       </c>
       <c r="B3">
-        <f>SUBTOTAL(109,B2:B2)</f>
         <v>949</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
+        <f>SUBTOTAL(109,A2:A3)</f>
+        <v>1000</v>
+      </c>
+      <c r="B4">
+        <f>SUBTOTAL(109,B2:B3)</f>
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
         <f>Table167[[#Totals],[Glob of Ectoplasm (Silverfed)]]/Table167[[#Totals],[Glob of Ectoplasm (Silverfed)]]</f>
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <f>Table167[[#Totals],[Pile of Crystalline Dust]]/Table167[[#Totals],[Glob of Ectoplasm (Silverfed)]]</f>
-        <v>1.8979999999999999</v>
+        <v>1.8680000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1139,11 +1305,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1181,108 +1345,131 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C2">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="D2">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="E2">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G2">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>12</v>
       </c>
       <c r="D3">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E3">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G3">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>SUBTOTAL(109,A2:A3)</f>
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="B4">
-        <f>SUBTOTAL(109,B2:B3)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <f>SUBTOTAL(109,C2:C3)</f>
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D4">
-        <f>SUBTOTAL(109,D2:D3)</f>
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="E4">
-        <f>SUBTOTAL(109,E2:E3)</f>
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="F4">
-        <f>SUBTOTAL(109,F2:F3)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <f>SUBTOTAL(109,G2:G3)</f>
-        <v>23</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
+        <f t="shared" ref="A5:G5" si="0">SUBTOTAL(109,A2:A4)</f>
+        <v>135</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>87</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
         <f>Table1678[[#Totals],[Reclaimed Wood Chunk (Copperfed)]]/Table1678[[#Totals],[Reclaimed Wood Chunk (Copperfed)]]</f>
         <v>1</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <f>Table1678[[#Totals],[Green Wood Log]]/Table1678[[#Totals],[Reclaimed Wood Chunk (Copperfed)]]</f>
-        <v>8.1967213114754092E-2</v>
-      </c>
-      <c r="C5">
+        <v>0.12592592592592591</v>
+      </c>
+      <c r="C6">
         <f>Table1678[[#Totals],[Soft Wood Logs]]/Table1678[[#Totals],[Reclaimed Wood Chunk (Copperfed)]]</f>
-        <v>0.39344262295081966</v>
-      </c>
-      <c r="D5">
+        <v>0.48148148148148145</v>
+      </c>
+      <c r="D6">
         <f>Table1678[[#Totals],[Seasoned Wood Logs]]/Table1678[[#Totals],[Reclaimed Wood Chunk (Copperfed)]]</f>
-        <v>0.4098360655737705</v>
-      </c>
-      <c r="E5">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="E6">
         <f>Table1678[[#Totals],[Hard Wood Logs]]/Table1678[[#Totals],[Reclaimed Wood Chunk (Copperfed)]]</f>
-        <v>0.67213114754098358</v>
-      </c>
-      <c r="F5">
+        <v>0.64444444444444449</v>
+      </c>
+      <c r="F6">
         <f>Table1678[[#Totals],[Elder Wood Logs ]]/Table1678[[#Totals],[Reclaimed Wood Chunk (Copperfed)]]</f>
-        <v>4.9180327868852458E-2</v>
-      </c>
-      <c r="G5">
+        <v>8.8888888888888892E-2</v>
+      </c>
+      <c r="G6">
         <f>Table1678[[#Totals],[Ancient Wood Logs]]/Table1678[[#Totals],[Reclaimed Wood Chunk (Copperfed)]]</f>
-        <v>0.37704918032786883</v>
+        <v>0.32592592592592595</v>
       </c>
     </row>
   </sheetData>
@@ -1298,9 +1485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE4A669-CD5A-41EF-92A4-0FB02C8F503F}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1370,127 +1555,115 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33DBE2BB-4C54-418B-A23E-EC9B0B3C4D5D}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C44" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="77.28515625" customWidth="1"/>
-    <col min="2" max="2" width="62.140625" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" customWidth="1"/>
-    <col min="4" max="4" width="32" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" customWidth="1"/>
-    <col min="6" max="6" width="29.140625" customWidth="1"/>
-    <col min="7" max="7" width="39.5703125" customWidth="1"/>
+    <col min="2" max="3" width="62.140625" customWidth="1"/>
+    <col min="4" max="4" width="34.5703125" customWidth="1"/>
+    <col min="5" max="5" width="32" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" customWidth="1"/>
+    <col min="8" max="8" width="39.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
       <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1088</v>
-      </c>
-      <c r="B2">
-        <v>44</v>
-      </c>
-      <c r="C2">
-        <v>51</v>
-      </c>
-      <c r="D2">
-        <v>57</v>
-      </c>
-      <c r="E2">
-        <v>15</v>
-      </c>
-      <c r="F2">
-        <v>534</v>
-      </c>
-      <c r="G2">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>SUBTOTAL(109,A2:A2)</f>
-        <v>1088</v>
+        <v>0</v>
       </c>
       <c r="B3">
         <f>SUBTOTAL(109,B2:B2)</f>
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:G3" si="0">SUBTOTAL(109,C2:C2)</f>
-        <v>51</v>
+        <f>SUBTOTAL(109,C2:C2)</f>
+        <v>0</v>
       </c>
       <c r="D3">
-        <f t="shared" si="0"/>
-        <v>57</v>
+        <f>SUBTOTAL(109,D2:D2)</f>
+        <v>0</v>
       </c>
       <c r="E3">
-        <f t="shared" si="0"/>
-        <v>15</v>
+        <f>SUBTOTAL(109,E2:E2)</f>
+        <v>0</v>
       </c>
       <c r="F3">
-        <f t="shared" si="0"/>
-        <v>534</v>
+        <f>SUBTOTAL(109,F2:F2)</f>
+        <v>0</v>
       </c>
       <c r="G3">
-        <f t="shared" si="0"/>
-        <v>636</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
+        <f>SUBTOTAL(109,G2:G2)</f>
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f>SUBTOTAL(109,H2:H2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="e">
         <f>Table16784[[#Totals],[Bloodstone-Warped Hides (Silverfed)]]/Table16784[[#Totals],[Bloodstone-Warped Hides (Silverfed)]]</f>
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <f>Table16784[[#Totals],[Rawhide Leather Sections]]/Table16784[[#Totals],[Bloodstone-Warped Hides (Silverfed)]]</f>
-        <v>4.0441176470588237E-2</v>
-      </c>
-      <c r="C4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="B4" t="e">
+        <f>Table16784[[#Totals],[Bloodstone-Warped Hides (Silverfed)2]]/Table16784[[#Totals],[Bloodstone-Warped Hides (Silverfed)]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C4" t="e">
+        <f>Table16784[[#Totals],[Coarse Leather Sections]]/Table16784[[#Totals],[Bloodstone-Warped Hides (Silverfed)]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D4" t="e">
         <f>Table16784[[#Totals],[Thin Leather Sections]]/Table16784[[#Totals],[Bloodstone-Warped Hides (Silverfed)]]</f>
-        <v>4.6875E-2</v>
-      </c>
-      <c r="D4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E4" t="e">
         <f>Table16784[[#Totals],[Rugged Leather Sections]]/Table16784[[#Totals],[Bloodstone-Warped Hides (Silverfed)]]</f>
-        <v>5.2389705882352942E-2</v>
-      </c>
-      <c r="E4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F4" t="e">
         <f>Table16784[[#Totals],[Hard Wood Logs]]/Table16784[[#Totals],[Bloodstone-Warped Hides (Silverfed)]]</f>
-        <v>1.3786764705882353E-2</v>
-      </c>
-      <c r="F4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G4" t="e">
         <f>Table16784[[#Totals],[Thick Leather Sections]]/Table16784[[#Totals],[Bloodstone-Warped Hides (Silverfed)]]</f>
-        <v>0.49080882352941174</v>
-      </c>
-      <c r="G4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H4" t="e">
         <f>Table16784[[#Totals],[Hardened Leather Sections]]/Table16784[[#Totals],[Bloodstone-Warped Hides (Silverfed)]]</f>
-        <v>0.5845588235294118</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
@@ -1503,11 +1676,9 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B14C73-549D-48E9-BC9A-B9258BD5715C}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B43" sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1521,16 +1692,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>27</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>28</v>
-      </c>
-      <c r="D1" t="s">
-        <v>29</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -1541,74 +1712,94 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>426</v>
+        <v>761</v>
       </c>
       <c r="B2">
-        <v>74</v>
+        <v>114</v>
       </c>
       <c r="C2">
-        <v>402</v>
+        <v>760</v>
       </c>
       <c r="D2">
-        <v>212</v>
+        <v>326</v>
       </c>
       <c r="E2">
-        <v>43</v>
+        <v>124</v>
       </c>
       <c r="F2">
-        <v>126</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>SUBTOTAL(109,A2:A2)</f>
         <v>426</v>
       </c>
       <c r="B3">
-        <f>SUBTOTAL(109,B2:B2)</f>
         <v>74</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:F3" si="0">SUBTOTAL(109,C2:C2)</f>
         <v>402</v>
       </c>
       <c r="D3">
-        <f t="shared" si="0"/>
         <v>212</v>
       </c>
       <c r="E3">
-        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="F3">
-        <f t="shared" si="0"/>
         <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
+        <f t="shared" ref="A4:F4" si="0">SUBTOTAL(109,A2:A3)</f>
+        <v>1187</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>188</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>1162</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>538</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>167</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>366</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
         <f>Table1678414[[#Totals],[Unstable Metal Chunks (Copperfed)]]/Table1678414[[#Totals],[Unstable Metal Chunks (Copperfed)]]</f>
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <f>Table1678414[[#Totals],[Copper Ore]]/Table1678414[[#Totals],[Unstable Metal Chunks (Copperfed)]]</f>
-        <v>0.17370892018779344</v>
-      </c>
-      <c r="C4">
+        <v>0.15838247683235046</v>
+      </c>
+      <c r="C5">
         <f>Table1678414[[#Totals],[Iron Ore]]/Table1678414[[#Totals],[Unstable Metal Chunks (Copperfed)]]</f>
-        <v>0.94366197183098588</v>
-      </c>
-      <c r="D4">
+        <v>0.97893850042122998</v>
+      </c>
+      <c r="D5">
         <f>Table1678414[[#Totals],[Platinum Ore]]/Table1678414[[#Totals],[Unstable Metal Chunks (Copperfed)]]</f>
-        <v>0.49765258215962443</v>
-      </c>
-      <c r="E4">
+        <v>0.45324347093513057</v>
+      </c>
+      <c r="E5">
         <f>Table1678414[[#Totals],[Mithril Ore]]/Table1678414[[#Totals],[Unstable Metal Chunks (Copperfed)]]</f>
-        <v>0.10093896713615023</v>
-      </c>
-      <c r="F4">
+        <v>0.14069081718618365</v>
+      </c>
+      <c r="F5">
         <f>Table1678414[[#Totals],[Orichalcum Ore]]/Table1678414[[#Totals],[Unstable Metal Chunks (Copperfed)]]</f>
-        <v>0.29577464788732394</v>
+        <v>0.30834035383319292</v>
       </c>
     </row>
   </sheetData>
@@ -1621,112 +1812,147 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FD039B-3C36-4A08-94BD-647B1301CE1A}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="77.28515625" customWidth="1"/>
     <col min="2" max="2" width="62.140625" customWidth="1"/>
     <col min="3" max="3" width="34.5703125" customWidth="1"/>
-    <col min="4" max="4" width="32" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" customWidth="1"/>
-    <col min="6" max="6" width="29.140625" customWidth="1"/>
+    <col min="4" max="5" width="32" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>31</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>32</v>
       </c>
-      <c r="D1" t="s">
-        <v>33</v>
-      </c>
       <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>85</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>359</v>
+      </c>
+      <c r="G2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>22</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="E2">
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
         <v>86</v>
       </c>
-      <c r="F2">
+      <c r="G3">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f>SUBTOTAL(109,A2:A2)</f>
-        <v>22</v>
-      </c>
-      <c r="B3">
-        <f>SUBTOTAL(109,B2:B2)</f>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:G4" si="0">SUBTOTAL(109,A2:A3)</f>
+        <v>107</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C3">
-        <f t="shared" ref="C3:F3" si="0">SUBTOTAL(109,C2:C2)</f>
-        <v>1</v>
-      </c>
-      <c r="D3">
+      <c r="D4">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E3">
+        <v>7</v>
+      </c>
+      <c r="E4">
         <f t="shared" si="0"/>
-        <v>86</v>
-      </c>
-      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="F4">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
+        <v>445</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
         <f>Table167841415[[#Totals],[Salvageable Fused Metal Scraps (Copperfed)]]/Table167841415[[#Totals],[Salvageable Fused Metal Scraps (Copperfed)]]</f>
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <f>Table167841415[[#Totals],[Molten Core]]/Table167841415[[#Totals],[Salvageable Fused Metal Scraps (Copperfed)]]</f>
-        <v>4.5454545454545456E-2</v>
-      </c>
-      <c r="C4">
+        <v>3.7383177570093455E-2</v>
+      </c>
+      <c r="C5">
         <f>Table167841415[[#Totals],[Molten Lodestone]]/Table167841415[[#Totals],[Salvageable Fused Metal Scraps (Copperfed)]]</f>
-        <v>4.5454545454545456E-2</v>
-      </c>
-      <c r="D4">
+        <v>9.3457943925233638E-3</v>
+      </c>
+      <c r="D5">
         <f>Table167841415[[#Totals],[Glacial Core]]/Table167841415[[#Totals],[Salvageable Fused Metal Scraps (Copperfed)]]</f>
-        <v>9.0909090909090912E-2</v>
-      </c>
-      <c r="E4">
+        <v>6.5420560747663545E-2</v>
+      </c>
+      <c r="E5">
+        <f>Table167841415[[#Totals],[Glacial Lodestone]]/Table167841415[[#Totals],[Salvageable Fused Metal Scraps (Copperfed)]]</f>
+        <v>2.8037383177570093E-2</v>
+      </c>
+      <c r="F5">
         <f>Table167841415[[#Totals],[Mithril Ore]]/Table167841415[[#Totals],[Salvageable Fused Metal Scraps (Copperfed)]]</f>
-        <v>3.9090909090909092</v>
-      </c>
-      <c r="F4">
+        <v>4.1588785046728969</v>
+      </c>
+      <c r="G5">
         <f>Table167841415[[#Totals],[Orichalcum Ore]]/Table167841415[[#Totals],[Salvageable Fused Metal Scraps (Copperfed)]]</f>
-        <v>0.27272727272727271</v>
+        <v>0.28037383177570091</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix for new dyes
</commit_message>
<xml_diff>
--- a/GW2Tradz/GW2Tradz/salvage.xlsx
+++ b/GW2Tradz/GW2Tradz/salvage.xlsx
@@ -8,23 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krise\Documents\GitHub\GW2Tradz\GW2Tradz\GW2Tradz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8B8ACB-E90F-498F-95EE-B4B3A31F5A46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB05404D-B061-4A30-9F05-15E14E8EB3EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="1000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="1000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valuable Metal Scrap (Copperfed" sheetId="1" r:id="rId1"/>
     <sheet name="Salvageable Intact Forged Scrap" sheetId="2" r:id="rId2"/>
-    <sheet name="Lump of Raw Ambrite (Copperfed)" sheetId="3" r:id="rId3"/>
-    <sheet name="Glob of Ectoplasm (Silverfed)" sheetId="4" r:id="rId4"/>
-    <sheet name="Reclaimed Wood Chunk (Copperfed" sheetId="5" r:id="rId5"/>
-    <sheet name="Discarded Garments (Copperfed)" sheetId="6" r:id="rId6"/>
-    <sheet name="Bloodstone-Warped Hides (Silver" sheetId="7" r:id="rId7"/>
-    <sheet name="Unstable Metal Chunks (Copperfe" sheetId="10" r:id="rId8"/>
-    <sheet name="Salvageable Fused Metal Scraps " sheetId="11" r:id="rId9"/>
-    <sheet name="Salvageable Metal Scraps (Coppe" sheetId="12" r:id="rId10"/>
-    <sheet name="Hard Leather Straps (Silverfed)" sheetId="9" r:id="rId11"/>
-    <sheet name="Hard Leather Straps (Copperfed)" sheetId="13" r:id="rId12"/>
+    <sheet name="s" sheetId="14" r:id="rId3"/>
+    <sheet name="Lump of Raw Ambrite (Copperfed)" sheetId="3" r:id="rId4"/>
+    <sheet name="Glob of Ectoplasm (Silverfed)" sheetId="4" r:id="rId5"/>
+    <sheet name="Reclaimed Wood Chunk (Copperfed" sheetId="5" r:id="rId6"/>
+    <sheet name="Discarded Garments (Copperfed)" sheetId="6" r:id="rId7"/>
+    <sheet name="Bloodstone-Warped Hides (Silver" sheetId="7" r:id="rId8"/>
+    <sheet name="Unstable Metal Chunks (Copperfe" sheetId="10" r:id="rId9"/>
+    <sheet name="Salvageable Fused Metal Scraps " sheetId="11" r:id="rId10"/>
+    <sheet name="Salvageable Metal Scraps (Coppe" sheetId="12" r:id="rId11"/>
+    <sheet name="Hard Leather Straps (Silverfed)" sheetId="9" r:id="rId12"/>
+    <sheet name="Hard Leather Straps (Copperfed)" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t>Orichalcum Ore</t>
   </si>
@@ -156,6 +157,9 @@
   </si>
   <si>
     <t>Hard Leather Straps (Copperfed)</t>
+  </si>
+  <si>
+    <t>Salvageable Aetherized Metal Scrap (Copperfed)</t>
   </si>
 </sst>
 </file>
@@ -235,6 +239,36 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{8CE988A0-C50E-4CC4-88CD-D3F5FB332B81}" name="Table167841415" displayName="Table167841415" ref="A1:G5" totalsRowCount="1">
+  <autoFilter ref="A1:G4" xr:uid="{7CCC29B3-4E29-4434-9033-BB5CD6A1C02E}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{21B805E5-8EF4-4B33-B45E-03CB622F6AD3}" name="Salvageable Fused Metal Scraps (Copperfed)" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(109,A2:A4)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{28F7B35D-F3F2-4F5D-A14A-5C0A1E59AB96}" name="Molten Core" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(109,B2:B4)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{62CCA669-CBD2-4DE6-84EC-17BB481C9C91}" name="Molten Lodestone" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(109,C2:C4)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{9556E610-E477-4966-A066-9B2695745F6E}" name="Glacial Core" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(109,D2:D4)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{80E8700E-CFC1-4F90-8331-94C026EE1108}" name="Glacial Lodestone" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(109,E2:E4)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{F1F3AD18-1C24-4218-9CCF-1CD3124E3CB8}" name="Mithril Ore" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(109,F2:F4)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{5C8FFD83-4405-4639-8D5C-AA0C78802CFF}" name="Orichalcum Ore" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(109,G2:G4)</totalsRowFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{E5E7FB19-106A-4512-B469-28100BDD1999}" name="Table16784141516" displayName="Table16784141516" ref="A1:C6" totalsRowCount="1">
   <autoFilter ref="A1:C5" xr:uid="{E1E674C0-644D-4043-A0DA-8F6C9A034074}"/>
   <tableColumns count="3">
@@ -252,7 +286,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{436DD24B-6473-49CB-BC2B-2C5E70B741F9}" name="Table167849" displayName="Table167849" ref="A1:C5" totalsRowCount="1">
   <autoFilter ref="A1:C4" xr:uid="{435B9412-207A-46D7-85DB-63D3D0B190BE}"/>
   <tableColumns count="3">
@@ -270,7 +304,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{A5A9E304-F35F-471C-81FA-4EDF4763158A}" name="Table16784910" displayName="Table16784910" ref="A1:C3" totalsRowCount="1">
   <autoFilter ref="A1:C2" xr:uid="{05916349-3643-410E-BD0E-4C40DC3B4DFA}"/>
   <tableColumns count="3">
@@ -289,20 +323,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table15" displayName="Table15" ref="A1:D8" totalsRowCount="1">
-  <autoFilter ref="A1:D7" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table15" displayName="Table15" ref="A1:D9" totalsRowCount="1">
+  <autoFilter ref="A1:D8" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Salvageable Intact Forged Scrap (Copperfed)" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,A2:A7)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,A2:A8)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Mithril Ore" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,B2:B7)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,B2:B8)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Orichalcum Ore" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,C2:C7)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,C2:C8)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Slivers of Twisting Forgemetal" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,D2:D7)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,D2:D8)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -310,6 +344,27 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6DF380B5-C9F7-4E43-9178-E6C8E703B27E}" name="Table1511" displayName="Table1511" ref="A1:D9" totalsRowCount="1">
+  <autoFilter ref="A1:D8" xr:uid="{1DCA64DF-36A2-4776-9848-2BF207CB0D4A}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{C8920653-4432-44AA-B867-97D18BF9907E}" name="Salvageable Aetherized Metal Scrap (Copperfed)" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(109,A2:A8)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{37C89639-242E-4183-8E73-B9A8AB1B9CA5}" name="Mithril Ore" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(109,B2:B8)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{EBA472C3-2636-479C-A1F4-F326E0D2D2E6}" name="Orichalcum Ore" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(109,C2:C8)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{79C33FB6-8130-425D-BF1A-2FBB66B67620}" name="Slivers of Twisting Forgemetal" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(109,D2:D8)</totalsRowFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table16" displayName="Table16" ref="A1:B4" totalsRowCount="1">
   <autoFilter ref="A1:B3" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="2">
@@ -324,22 +379,22 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table167" displayName="Table167" ref="A1:B7" totalsRowCount="1">
-  <autoFilter ref="A1:B6" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table167" displayName="Table167" ref="A1:B8" totalsRowCount="1">
+  <autoFilter ref="A1:B7" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Glob of Ectoplasm (Silverfed)" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,A2:A6)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,A2:A7)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Pile of Crystalline Dust" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,B2:B6)</totalsRowFormula>
+      <totalsRowFormula>SUBTOTAL(109,B2:B7)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table1678" displayName="Table1678" ref="A1:G7" totalsRowCount="1">
   <autoFilter ref="A1:G6" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="7">
@@ -369,7 +424,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1E3207A3-E09A-411C-A707-91A061A3D0E8}" name="Table16783" displayName="Table16783" ref="A1:C3" totalsRowCount="1">
   <autoFilter ref="A1:C2" xr:uid="{956112EF-C722-411C-A2E0-E9E17536B520}"/>
   <tableColumns count="3">
@@ -387,7 +442,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6683A40A-984F-4C8C-B5BD-CEDCA44A00C1}" name="Table16784" displayName="Table16784" ref="A1:G4" totalsRowCount="1">
   <autoFilter ref="A1:G3" xr:uid="{25A4AE94-A8F7-4B52-994F-DE080FA22BF0}"/>
   <tableColumns count="7">
@@ -417,7 +472,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{5DA2CE26-8E50-4E72-9C9C-77AF18B12840}" name="Table1678414" displayName="Table1678414" ref="A1:F6" totalsRowCount="1">
   <autoFilter ref="A1:F5" xr:uid="{161BA580-722A-410D-8E2D-E64F92884D13}"/>
   <tableColumns count="6">
@@ -438,36 +493,6 @@
     </tableColumn>
     <tableColumn id="7" xr3:uid="{0C6CECE8-CF3F-4FD2-BCB2-8948DCAAE7D6}" name="Orichalcum Ore" totalsRowFunction="custom">
       <totalsRowFormula>SUBTOTAL(109,F2:F5)</totalsRowFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{8CE988A0-C50E-4CC4-88CD-D3F5FB332B81}" name="Table167841415" displayName="Table167841415" ref="A1:G5" totalsRowCount="1">
-  <autoFilter ref="A1:G4" xr:uid="{7CCC29B3-4E29-4434-9033-BB5CD6A1C02E}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{21B805E5-8EF4-4B33-B45E-03CB622F6AD3}" name="Salvageable Fused Metal Scraps (Copperfed)" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,A2:A4)</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="2" xr3:uid="{28F7B35D-F3F2-4F5D-A14A-5C0A1E59AB96}" name="Molten Core" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,B2:B4)</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{62CCA669-CBD2-4DE6-84EC-17BB481C9C91}" name="Molten Lodestone" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,C2:C4)</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{9556E610-E477-4966-A066-9B2695745F6E}" name="Glacial Core" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,D2:D4)</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{80E8700E-CFC1-4F90-8331-94C026EE1108}" name="Glacial Lodestone" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,E2:E4)</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{F1F3AD18-1C24-4218-9CCF-1CD3124E3CB8}" name="Mithril Ore" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,F2:F4)</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{5C8FFD83-4405-4639-8D5C-AA0C78802CFF}" name="Orichalcum Ore" totalsRowFunction="custom">
-      <totalsRowFormula>SUBTOTAL(109,G2:G4)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -932,6 +957,184 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FD039B-3C36-4A08-94BD-647B1301CE1A}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="77.28515625" customWidth="1"/>
+    <col min="2" max="2" width="62.140625" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" customWidth="1"/>
+    <col min="4" max="5" width="32" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>349</v>
+      </c>
+      <c r="B2">
+        <v>21</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>19</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <v>1454</v>
+      </c>
+      <c r="G2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>85</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>359</v>
+      </c>
+      <c r="G3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>86</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" ref="A5:G5" si="0">SUBTOTAL(109,A2:A4)</f>
+        <v>456</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>1899</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f>Table167841415[[#Totals],[Salvageable Fused Metal Scraps (Copperfed)]]/Table167841415[[#Totals],[Salvageable Fused Metal Scraps (Copperfed)]]</f>
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <f>Table167841415[[#Totals],[Molten Core]]/Table167841415[[#Totals],[Salvageable Fused Metal Scraps (Copperfed)]]</f>
+        <v>5.4824561403508769E-2</v>
+      </c>
+      <c r="C6">
+        <f>Table167841415[[#Totals],[Molten Lodestone]]/Table167841415[[#Totals],[Salvageable Fused Metal Scraps (Copperfed)]]</f>
+        <v>8.771929824561403E-3</v>
+      </c>
+      <c r="D6">
+        <f>Table167841415[[#Totals],[Glacial Core]]/Table167841415[[#Totals],[Salvageable Fused Metal Scraps (Copperfed)]]</f>
+        <v>5.701754385964912E-2</v>
+      </c>
+      <c r="E6">
+        <f>Table167841415[[#Totals],[Glacial Lodestone]]/Table167841415[[#Totals],[Salvageable Fused Metal Scraps (Copperfed)]]</f>
+        <v>1.9736842105263157E-2</v>
+      </c>
+      <c r="F6">
+        <f>Table167841415[[#Totals],[Mithril Ore]]/Table167841415[[#Totals],[Salvageable Fused Metal Scraps (Copperfed)]]</f>
+        <v>4.1644736842105265</v>
+      </c>
+      <c r="G6">
+        <f>Table167841415[[#Totals],[Orichalcum Ore]]/Table167841415[[#Totals],[Salvageable Fused Metal Scraps (Copperfed)]]</f>
+        <v>0.26315789473684209</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF5987D4-1F44-4781-96D3-48B6972FA2CE}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -1037,7 +1240,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C72D2860-57B6-4373-880B-086D8C6F9373}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -1132,7 +1335,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB5B8851-65C4-4571-BF3E-34CCB99B2EA2}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1207,10 +1410,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,52 +1510,66 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>491</v>
+        <v>28</v>
       </c>
       <c r="B7">
-        <v>2061</v>
+        <v>137</v>
       </c>
       <c r="C7">
-        <v>147</v>
+        <v>9</v>
       </c>
       <c r="D7">
-        <v>118</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f>SUBTOTAL(109,A2:A7)</f>
-        <v>3382</v>
+        <v>491</v>
       </c>
       <c r="B8">
-        <f>SUBTOTAL(109,B2:B7)</f>
-        <v>14258</v>
+        <v>2061</v>
       </c>
       <c r="C8">
-        <f>SUBTOTAL(109,C2:C7)</f>
-        <v>1026</v>
+        <v>147</v>
       </c>
       <c r="D8">
-        <f>SUBTOTAL(109,D2:D7)</f>
-        <v>873</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
+        <f>SUBTOTAL(109,A2:A8)</f>
+        <v>3410</v>
+      </c>
+      <c r="B9">
+        <f>SUBTOTAL(109,B2:B8)</f>
+        <v>14395</v>
+      </c>
+      <c r="C9">
+        <f>SUBTOTAL(109,C2:C8)</f>
+        <v>1035</v>
+      </c>
+      <c r="D9">
+        <f>SUBTOTAL(109,D2:D8)</f>
+        <v>875</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
         <f>Table15[[#Totals],[Salvageable Intact Forged Scrap (Copperfed)]]/Table15[[#Totals],[Salvageable Intact Forged Scrap (Copperfed)]]</f>
         <v>1</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <f>Table15[[#Totals],[Mithril Ore]]/Table15[[#Totals],[Salvageable Intact Forged Scrap (Copperfed)]]</f>
-        <v>4.2158486102897692</v>
-      </c>
-      <c r="C9">
+        <v>4.2214076246334313</v>
+      </c>
+      <c r="C10">
         <f>Table15[[#Totals],[Orichalcum Ore]]/Table15[[#Totals],[Salvageable Intact Forged Scrap (Copperfed)]]</f>
-        <v>0.30337078651685395</v>
-      </c>
-      <c r="D9">
+        <v>0.30351906158357772</v>
+      </c>
+      <c r="D10">
         <f>Table15[[#Totals],[Slivers of Twisting Forgemetal]]/Table15[[#Totals],[Salvageable Intact Forged Scrap (Copperfed)]]</f>
-        <v>0.25813128326434065</v>
+        <v>0.25659824046920821</v>
       </c>
     </row>
   </sheetData>
@@ -1364,6 +1581,176 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44D03BF8-91B7-43D8-94EE-9FAD88BBDB34}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.7109375" customWidth="1"/>
+    <col min="2" max="2" width="57.42578125" customWidth="1"/>
+    <col min="3" max="3" width="64.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>223</v>
+      </c>
+      <c r="B2">
+        <v>982</v>
+      </c>
+      <c r="C2">
+        <v>57</v>
+      </c>
+      <c r="D2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>518</v>
+      </c>
+      <c r="B3">
+        <v>2169</v>
+      </c>
+      <c r="C3">
+        <v>150</v>
+      </c>
+      <c r="D3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>346</v>
+      </c>
+      <c r="B4">
+        <v>1503</v>
+      </c>
+      <c r="C4">
+        <v>117</v>
+      </c>
+      <c r="D4">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1482</v>
+      </c>
+      <c r="B5">
+        <v>6188</v>
+      </c>
+      <c r="C5">
+        <v>438</v>
+      </c>
+      <c r="D5">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>322</v>
+      </c>
+      <c r="B6">
+        <v>1355</v>
+      </c>
+      <c r="C6">
+        <v>117</v>
+      </c>
+      <c r="D6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>28</v>
+      </c>
+      <c r="B7">
+        <v>137</v>
+      </c>
+      <c r="C7">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>491</v>
+      </c>
+      <c r="B8">
+        <v>2061</v>
+      </c>
+      <c r="C8">
+        <v>147</v>
+      </c>
+      <c r="D8">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>SUBTOTAL(109,A2:A8)</f>
+        <v>3410</v>
+      </c>
+      <c r="B9">
+        <f>SUBTOTAL(109,B2:B8)</f>
+        <v>14395</v>
+      </c>
+      <c r="C9">
+        <f>SUBTOTAL(109,C2:C8)</f>
+        <v>1035</v>
+      </c>
+      <c r="D9">
+        <f>SUBTOTAL(109,D2:D8)</f>
+        <v>875</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f>Table1511[[#Totals],[Salvageable Aetherized Metal Scrap (Copperfed)]]/Table1511[[#Totals],[Salvageable Aetherized Metal Scrap (Copperfed)]]</f>
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <f>Table1511[[#Totals],[Mithril Ore]]/Table1511[[#Totals],[Salvageable Aetherized Metal Scrap (Copperfed)]]</f>
+        <v>4.2214076246334313</v>
+      </c>
+      <c r="C10">
+        <f>Table1511[[#Totals],[Orichalcum Ore]]/Table1511[[#Totals],[Salvageable Aetherized Metal Scrap (Copperfed)]]</f>
+        <v>0.30351906158357772</v>
+      </c>
+      <c r="D10">
+        <f>Table1511[[#Totals],[Slivers of Twisting Forgemetal]]/Table1511[[#Totals],[Salvageable Aetherized Metal Scrap (Copperfed)]]</f>
+        <v>0.25659824046920821</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1427,12 +1814,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="A5:XFD5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1475,38 +1862,46 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1000</v>
+        <v>3500</v>
       </c>
       <c r="B5">
-        <v>1878</v>
+        <v>6464</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="B6">
-        <v>949</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>SUBTOTAL(109,A2:A6)</f>
-        <v>2647</v>
+        <v>500</v>
       </c>
       <c r="B7">
-        <f>SUBTOTAL(109,B2:B6)</f>
-        <v>4977</v>
+        <v>949</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
+        <f>SUBTOTAL(109,A2:A7)</f>
+        <v>6147</v>
+      </c>
+      <c r="B8">
+        <f>SUBTOTAL(109,B2:B7)</f>
+        <v>11441</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
         <f>Table167[[#Totals],[Glob of Ectoplasm (Silverfed)]]/Table167[[#Totals],[Glob of Ectoplasm (Silverfed)]]</f>
         <v>1</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <f>Table167[[#Totals],[Pile of Crystalline Dust]]/Table167[[#Totals],[Glob of Ectoplasm (Silverfed)]]</f>
-        <v>1.8802417831507368</v>
+        <v>1.861233121848056</v>
       </c>
     </row>
   </sheetData>
@@ -1517,7 +1912,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -1743,7 +2138,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE4A669-CD5A-41EF-92A4-0FB02C8F503F}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1815,7 +2210,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33DBE2BB-4C54-418B-A23E-EC9B0B3C4D5D}">
   <dimension ref="A1:G5"/>
   <sheetViews>
@@ -1970,7 +2365,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B14C73-549D-48E9-BC9A-B9258BD5715C}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -2146,182 +2541,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FD039B-3C36-4A08-94BD-647B1301CE1A}">
-  <dimension ref="A1:G6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="77.28515625" customWidth="1"/>
-    <col min="2" max="2" width="62.140625" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" customWidth="1"/>
-    <col min="4" max="5" width="32" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" customWidth="1"/>
-    <col min="7" max="7" width="29.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>349</v>
-      </c>
-      <c r="B2">
-        <v>21</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>19</v>
-      </c>
-      <c r="E2">
-        <v>6</v>
-      </c>
-      <c r="F2">
-        <v>1454</v>
-      </c>
-      <c r="G2">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>85</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>359</v>
-      </c>
-      <c r="G3">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>22</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>86</v>
-      </c>
-      <c r="G4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f t="shared" ref="A5:G5" si="0">SUBTOTAL(109,A2:A4)</f>
-        <v>456</v>
-      </c>
-      <c r="B5">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="C5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="0"/>
-        <v>1899</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f>Table167841415[[#Totals],[Salvageable Fused Metal Scraps (Copperfed)]]/Table167841415[[#Totals],[Salvageable Fused Metal Scraps (Copperfed)]]</f>
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <f>Table167841415[[#Totals],[Molten Core]]/Table167841415[[#Totals],[Salvageable Fused Metal Scraps (Copperfed)]]</f>
-        <v>5.4824561403508769E-2</v>
-      </c>
-      <c r="C6">
-        <f>Table167841415[[#Totals],[Molten Lodestone]]/Table167841415[[#Totals],[Salvageable Fused Metal Scraps (Copperfed)]]</f>
-        <v>8.771929824561403E-3</v>
-      </c>
-      <c r="D6">
-        <f>Table167841415[[#Totals],[Glacial Core]]/Table167841415[[#Totals],[Salvageable Fused Metal Scraps (Copperfed)]]</f>
-        <v>5.701754385964912E-2</v>
-      </c>
-      <c r="E6">
-        <f>Table167841415[[#Totals],[Glacial Lodestone]]/Table167841415[[#Totals],[Salvageable Fused Metal Scraps (Copperfed)]]</f>
-        <v>1.9736842105263157E-2</v>
-      </c>
-      <c r="F6">
-        <f>Table167841415[[#Totals],[Mithril Ore]]/Table167841415[[#Totals],[Salvageable Fused Metal Scraps (Copperfed)]]</f>
-        <v>4.1644736842105265</v>
-      </c>
-      <c r="G6">
-        <f>Table167841415[[#Totals],[Orichalcum Ore]]/Table167841415[[#Totals],[Salvageable Fused Metal Scraps (Copperfed)]]</f>
-        <v>0.26315789473684209</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>